<commit_message>
Water split to HF-MF-LF, about to tweak to allow HORIBA (may break WITEC)
</commit_message>
<xml_diff>
--- a/docs/Examples/Example1b_CO2_Fluid_Inclusions/Calibration_fitting_w_sec_phases.xlsx
+++ b/docs/Examples/Example1b_CO2_Fluid_Inclusions/Calibration_fitting_w_sec_phases.xlsx
@@ -1,34 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25831"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\Berkeley_NEW\DiadFit_outer\docs\Examples\Example1b_CO2_Fluid_Inclusions\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{649C2039-770E-43FC-9FEF-8B4743696B13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029" iterate="1" concurrentCalc="0"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -391,8 +372,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -455,14 +436,6 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
@@ -509,7 +482,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -541,27 +514,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -593,24 +548,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -786,16 +723,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:BH17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:60" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:60">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -974,7 +909,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="2" spans="1:60" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:60">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -991,28 +926,28 @@
         <v>103.0572812069299</v>
       </c>
       <c r="F2">
-        <v>1286.0360781048551</v>
+        <v>1286.036078104855</v>
       </c>
       <c r="G2">
-        <v>590.18347754251386</v>
+        <v>590.1834775425139</v>
       </c>
       <c r="H2">
-        <v>1286.0360781048551</v>
+        <v>1286.036078104855</v>
       </c>
       <c r="I2">
-        <v>599.33863023707067</v>
+        <v>599.3386302370707</v>
       </c>
       <c r="J2">
-        <v>0.43521050642235298</v>
+        <v>0.435210506422353</v>
       </c>
       <c r="K2">
-        <v>4.0748769901688879</v>
+        <v>4.074876990168888</v>
       </c>
       <c r="L2">
-        <v>0.27285501612411461</v>
+        <v>0.2728550161241146</v>
       </c>
       <c r="M2">
-        <v>0.87042101284470597</v>
+        <v>0.870421012844706</v>
       </c>
       <c r="N2" t="s">
         <v>75</v>
@@ -1021,25 +956,25 @@
         <v>1389.093359311785</v>
       </c>
       <c r="P2">
-        <v>968.20598174724751</v>
+        <v>968.2059817472475</v>
       </c>
       <c r="Q2">
         <v>1389.093359311785</v>
       </c>
       <c r="R2">
-        <v>903.74846969156408</v>
+        <v>903.7484696915641</v>
       </c>
       <c r="S2">
-        <v>0.39553138635583301</v>
+        <v>0.395531386355833</v>
       </c>
       <c r="U2">
-        <v>3.7434356213393012</v>
+        <v>3.743435621339301</v>
       </c>
       <c r="V2">
-        <v>0.30605545520312488</v>
+        <v>0.3060554552031249</v>
       </c>
       <c r="W2">
-        <v>0.79106277271166592</v>
+        <v>0.7910627727116659</v>
       </c>
       <c r="X2" t="s">
         <v>75</v>
@@ -1078,7 +1013,7 @@
         <v>43795</v>
       </c>
       <c r="AZ2">
-        <v>1325.0039999999999</v>
+        <v>1325.004</v>
       </c>
       <c r="BA2">
         <v>0.9978450505721892</v>
@@ -1090,13 +1025,13 @@
         <v>1151.160658708769</v>
       </c>
       <c r="BD2">
-        <v>57.033468024938948</v>
+        <v>57.03346802493895</v>
       </c>
       <c r="BE2">
         <v>26.54027290352408</v>
       </c>
     </row>
-    <row r="3" spans="1:60" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:60">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -1110,58 +1045,58 @@
         <v>60</v>
       </c>
       <c r="E3">
-        <v>103.01065082298651</v>
+        <v>103.0106508229865</v>
       </c>
       <c r="F3">
-        <v>1286.1575007400329</v>
+        <v>1286.157500740033</v>
       </c>
       <c r="G3">
-        <v>227.28899772001711</v>
+        <v>227.2889977200171</v>
       </c>
       <c r="H3">
-        <v>1286.1575007400329</v>
+        <v>1286.157500740033</v>
       </c>
       <c r="I3">
-        <v>200.26682321118349</v>
+        <v>200.2668232111835</v>
       </c>
       <c r="J3">
         <v>0.4096980686129264</v>
       </c>
       <c r="K3">
-        <v>3.2811043585473358</v>
+        <v>3.281104358547336</v>
       </c>
       <c r="L3">
-        <v>2.195236324449212E-2</v>
+        <v>0.02195236324449212</v>
       </c>
       <c r="M3">
-        <v>0.81939613722585281</v>
+        <v>0.8193961372258528</v>
       </c>
       <c r="N3" t="s">
         <v>75</v>
       </c>
       <c r="O3">
-        <v>1389.1681515630189</v>
+        <v>1389.168151563019</v>
       </c>
       <c r="P3">
-        <v>374.13853291395878</v>
+        <v>374.1385329139588</v>
       </c>
       <c r="Q3">
-        <v>1389.1681515630189</v>
+        <v>1389.168151563019</v>
       </c>
       <c r="R3">
-        <v>344.05986871633019</v>
+        <v>344.0598687163302</v>
       </c>
       <c r="S3">
-        <v>0.38815407218127967</v>
+        <v>0.3881540721812797</v>
       </c>
       <c r="U3">
-        <v>3.6227300308767969</v>
+        <v>3.622730030876797</v>
       </c>
       <c r="V3">
-        <v>0.31896488896817721</v>
+        <v>0.3189648889681772</v>
       </c>
       <c r="W3">
-        <v>0.77630814436255946</v>
+        <v>0.7763081443625595</v>
       </c>
       <c r="X3" t="s">
         <v>75</v>
@@ -1200,13 +1135,13 @@
         <v>44393</v>
       </c>
       <c r="AZ3">
-        <v>1325.0039999999999</v>
+        <v>1325.004</v>
       </c>
       <c r="BA3">
-        <v>0.99783737227149572</v>
+        <v>0.9978373722714957</v>
       </c>
     </row>
-    <row r="4" spans="1:60" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:60">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -1214,7 +1149,7 @@
         <v>0</v>
       </c>
       <c r="C4">
-        <v>102.82239006784501</v>
+        <v>102.822390067845</v>
       </c>
       <c r="D4" t="s">
         <v>61</v>
@@ -1223,28 +1158,28 @@
         <v>103.0461885476486</v>
       </c>
       <c r="F4">
-        <v>1286.0742355474999</v>
+        <v>1286.0742355475</v>
       </c>
       <c r="G4">
-        <v>570.01045090549599</v>
+        <v>570.010450905496</v>
       </c>
       <c r="H4">
-        <v>1286.0742355474999</v>
+        <v>1286.0742355475</v>
       </c>
       <c r="I4">
-        <v>580.89780468609456</v>
+        <v>580.8978046860946</v>
       </c>
       <c r="J4">
-        <v>0.42239735335506662</v>
+        <v>0.4223973533550666</v>
       </c>
       <c r="K4">
         <v>3.58537743345105</v>
       </c>
       <c r="L4">
-        <v>0.36386365924355107</v>
+        <v>0.3638636592435511</v>
       </c>
       <c r="M4">
-        <v>0.84479470671013313</v>
+        <v>0.8447947067101331</v>
       </c>
       <c r="N4" t="s">
         <v>75</v>
@@ -1253,25 +1188,25 @@
         <v>1389.120424095149</v>
       </c>
       <c r="P4">
-        <v>888.68584220524917</v>
+        <v>888.6858422052492</v>
       </c>
       <c r="Q4">
         <v>1389.120424095149</v>
       </c>
       <c r="R4">
-        <v>839.61978580701964</v>
+        <v>839.6197858070196</v>
       </c>
       <c r="S4">
-        <v>0.39962929919184548</v>
+        <v>0.3996292991918455</v>
       </c>
       <c r="U4">
-        <v>3.9224644607575261</v>
+        <v>3.922464460757526</v>
       </c>
       <c r="V4">
-        <v>0.31025981845089451</v>
+        <v>0.3102598184508945</v>
       </c>
       <c r="W4">
-        <v>0.79925859838369107</v>
+        <v>0.7992585983836911</v>
       </c>
       <c r="X4" t="s">
         <v>75</v>
@@ -1310,13 +1245,13 @@
         <v>45146</v>
       </c>
       <c r="AZ4">
-        <v>1325.0039999999999</v>
+        <v>1325.004</v>
       </c>
       <c r="BA4">
-        <v>0.99782817314295802</v>
+        <v>0.997828173142958</v>
       </c>
     </row>
-    <row r="5" spans="1:60" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:60">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -1336,49 +1271,49 @@
         <v>1285.431591413442</v>
       </c>
       <c r="G5">
-        <v>65.483824774253492</v>
+        <v>65.48382477425349</v>
       </c>
       <c r="H5">
         <v>1285.431591413442</v>
       </c>
       <c r="I5">
-        <v>81.303002371311621</v>
+        <v>81.30300237131162</v>
       </c>
       <c r="J5">
-        <v>0.57473651242942081</v>
+        <v>0.5747365124294208</v>
       </c>
       <c r="K5">
         <v>3.109908838780314</v>
       </c>
       <c r="L5">
-        <v>2.9271064294622559E-8</v>
+        <v>2.927106429462256E-08</v>
       </c>
       <c r="M5">
-        <v>1.1494730248588421</v>
+        <v>1.149473024858842</v>
       </c>
       <c r="N5" t="s">
         <v>75</v>
       </c>
       <c r="O5">
-        <v>1388.7421059547289</v>
+        <v>1388.742105954729</v>
       </c>
       <c r="P5">
-        <v>129.44748305814821</v>
+        <v>129.4474830581482</v>
       </c>
       <c r="Q5">
-        <v>1388.7421059547289</v>
+        <v>1388.742105954729</v>
       </c>
       <c r="R5">
-        <v>167.56512947040181</v>
+        <v>167.5651294704018</v>
       </c>
       <c r="S5">
-        <v>0.47906157906406049</v>
+        <v>0.4790615790640605</v>
       </c>
       <c r="U5">
-        <v>2.3909776955752751</v>
+        <v>2.390977695575275</v>
       </c>
       <c r="V5">
-        <v>0.66591320313734281</v>
+        <v>0.6659132031373428</v>
       </c>
       <c r="W5">
         <v>0.9581231581281211</v>
@@ -1420,13 +1355,13 @@
         <v>45944</v>
       </c>
       <c r="AZ5">
-        <v>1325.0039999999999</v>
+        <v>1325.004</v>
       </c>
       <c r="BA5">
         <v>0.9978189953195431</v>
       </c>
     </row>
-    <row r="6" spans="1:60" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:60">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -1446,25 +1381,25 @@
         <v>1285.435780646731</v>
       </c>
       <c r="G6">
-        <v>607.68867514271165</v>
+        <v>607.6886751427116</v>
       </c>
       <c r="H6">
         <v>1285.435780646731</v>
       </c>
       <c r="I6">
-        <v>895.51329940375479</v>
+        <v>895.5132994037548</v>
       </c>
       <c r="J6">
-        <v>0.56831616419291953</v>
+        <v>0.5683161641929195</v>
       </c>
       <c r="K6">
-        <v>3.5711870325871722</v>
+        <v>3.571187032587172</v>
       </c>
       <c r="L6">
-        <v>0.55539143846986128</v>
+        <v>0.5553914384698613</v>
       </c>
       <c r="M6">
-        <v>1.1366323283858391</v>
+        <v>1.136632328385839</v>
       </c>
       <c r="N6" t="s">
         <v>75</v>
@@ -1473,7 +1408,7 @@
         <v>1388.740377004782</v>
       </c>
       <c r="P6">
-        <v>1147.7468445434099</v>
+        <v>1147.74684454341</v>
       </c>
       <c r="Q6">
         <v>1388.740377004782</v>
@@ -1482,16 +1417,16 @@
         <v>1426.205692176087</v>
       </c>
       <c r="S6">
-        <v>0.48109036272197597</v>
+        <v>0.481090362721976</v>
       </c>
       <c r="U6">
-        <v>4.0560619222861929</v>
+        <v>4.056061922286193</v>
       </c>
       <c r="V6">
-        <v>0.54868613710150349</v>
+        <v>0.5486861371015035</v>
       </c>
       <c r="W6">
-        <v>0.96218072544395206</v>
+        <v>0.9621807254439521</v>
       </c>
       <c r="X6" t="s">
         <v>75</v>
@@ -1530,10 +1465,10 @@
         <v>46247</v>
       </c>
       <c r="AZ6">
-        <v>1325.0039999999999</v>
+        <v>1325.004</v>
       </c>
       <c r="BA6">
-        <v>0.99781566442592184</v>
+        <v>0.9978156644259218</v>
       </c>
       <c r="BB6" t="s">
         <v>80</v>
@@ -1542,13 +1477,13 @@
         <v>1090.889671208419</v>
       </c>
       <c r="BG6">
-        <v>868.25458451039231</v>
+        <v>868.2545845103923</v>
       </c>
       <c r="BH6">
-        <v>43.035082252189532</v>
+        <v>43.03508225218953</v>
       </c>
     </row>
-    <row r="7" spans="1:60" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:60">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -1574,7 +1509,7 @@
         <v>1285.310713133335</v>
       </c>
       <c r="I7">
-        <v>210.38802709169829</v>
+        <v>210.3880270916983</v>
       </c>
       <c r="J7">
         <v>0.6316854004922916</v>
@@ -1583,7 +1518,7 @@
         <v>1.715820019472321</v>
       </c>
       <c r="L7">
-        <v>0.61838028352969177</v>
+        <v>0.6183802835296918</v>
       </c>
       <c r="M7">
         <v>1.263370800984583</v>
@@ -1595,22 +1530,22 @@
         <v>1388.651808242689</v>
       </c>
       <c r="P7">
-        <v>235.75092169944921</v>
+        <v>235.7509216994492</v>
       </c>
       <c r="Q7">
         <v>1388.651808242689</v>
       </c>
       <c r="R7">
-        <v>317.85372184788628</v>
+        <v>317.8537218478863</v>
       </c>
       <c r="S7">
-        <v>0.53133883910793989</v>
+        <v>0.5313388391079399</v>
       </c>
       <c r="U7">
-        <v>1.7677045883756539</v>
+        <v>1.767704588375654</v>
       </c>
       <c r="V7">
-        <v>0.50551833387199629</v>
+        <v>0.5055183338719963</v>
       </c>
       <c r="W7">
         <v>1.06267767821588</v>
@@ -1652,25 +1587,25 @@
         <v>51532</v>
       </c>
       <c r="AZ7">
-        <v>1325.0039999999999</v>
+        <v>1325.004</v>
       </c>
       <c r="BA7">
-        <v>0.99777119202068276</v>
+        <v>0.9977711920206828</v>
       </c>
       <c r="BB7" t="s">
         <v>81</v>
       </c>
       <c r="BC7">
-        <v>1150.5918295469539</v>
+        <v>1150.591829546954</v>
       </c>
       <c r="BD7">
-        <v>81.865420848626457</v>
+        <v>81.86542084862646</v>
       </c>
       <c r="BE7">
-        <v>56.150040997841522</v>
+        <v>56.15004099784152</v>
       </c>
     </row>
-    <row r="8" spans="1:60" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:60">
       <c r="A8" s="1">
         <v>6</v>
       </c>
@@ -1684,28 +1619,28 @@
         <v>65</v>
       </c>
       <c r="E8">
-        <v>103.30103482851651</v>
+        <v>103.3010348285165</v>
       </c>
       <c r="F8">
         <v>1285.407603458091</v>
       </c>
       <c r="G8">
-        <v>520.81902407188682</v>
+        <v>520.8190240718868</v>
       </c>
       <c r="H8">
         <v>1285.407603458091</v>
       </c>
       <c r="I8">
-        <v>814.80557929779343</v>
+        <v>814.8055792977934</v>
       </c>
       <c r="J8">
-        <v>0.56238424143587862</v>
+        <v>0.5623842414358786</v>
       </c>
       <c r="K8">
-        <v>3.5982424662266599</v>
+        <v>3.59824246622666</v>
       </c>
       <c r="L8">
-        <v>0.73237396047629633</v>
+        <v>0.7323739604762963</v>
       </c>
       <c r="M8">
         <v>1.124768482871757</v>
@@ -1717,22 +1652,22 @@
         <v>1388.708638286608</v>
       </c>
       <c r="P8">
-        <v>938.39063895017023</v>
+        <v>938.3906389501702</v>
       </c>
       <c r="Q8">
         <v>1388.708638286608</v>
       </c>
       <c r="R8">
-        <v>1219.1098186888919</v>
+        <v>1219.109818688892</v>
       </c>
       <c r="S8">
-        <v>0.50756443500013237</v>
+        <v>0.5075644350001324</v>
       </c>
       <c r="U8">
         <v>3.674293975426854</v>
       </c>
       <c r="V8">
-        <v>0.52503334675602598</v>
+        <v>0.525033346756026</v>
       </c>
       <c r="W8">
         <v>1.015128870000265</v>
@@ -1774,25 +1709,25 @@
         <v>52872</v>
       </c>
       <c r="AZ8">
-        <v>1325.0039999999999</v>
+        <v>1325.004</v>
       </c>
       <c r="BA8">
-        <v>0.99776401207613441</v>
+        <v>0.9977640120761344</v>
       </c>
       <c r="BB8" t="s">
         <v>82</v>
       </c>
       <c r="BC8">
-        <v>1150.6428108593759</v>
+        <v>1150.642810859376</v>
       </c>
       <c r="BD8">
-        <v>374.15573107674129</v>
+        <v>374.1557310767413</v>
       </c>
       <c r="BE8">
-        <v>235.88333617828451</v>
+        <v>235.8833361782845</v>
       </c>
     </row>
-    <row r="9" spans="1:60" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:60">
       <c r="A9" s="1">
         <v>7</v>
       </c>
@@ -1800,7 +1735,7 @@
         <v>0</v>
       </c>
       <c r="C9">
-        <v>103.07099102081951</v>
+        <v>103.0709910208195</v>
       </c>
       <c r="D9" t="s">
         <v>66</v>
@@ -1812,52 +1747,52 @@
         <v>1285.362729075174</v>
       </c>
       <c r="G9">
-        <v>743.63097388886388</v>
+        <v>743.6309738888639</v>
       </c>
       <c r="H9">
         <v>1285.362729075174</v>
       </c>
       <c r="I9">
-        <v>1183.6710774289561</v>
+        <v>1183.671077428956</v>
       </c>
       <c r="J9">
-        <v>0.59187398997317664</v>
+        <v>0.5918739899731766</v>
       </c>
       <c r="K9">
-        <v>4.1963315585975254</v>
+        <v>4.196331558597525</v>
       </c>
       <c r="L9">
-        <v>0.64693163815498689</v>
+        <v>0.6469316381549869</v>
       </c>
       <c r="M9">
-        <v>1.1837479799463531</v>
+        <v>1.183747979946353</v>
       </c>
       <c r="N9" t="s">
         <v>75</v>
       </c>
       <c r="O9">
-        <v>1388.6655483178949</v>
+        <v>1388.665548317895</v>
       </c>
       <c r="P9">
-        <v>1382.7840611294009</v>
+        <v>1382.784061129401</v>
       </c>
       <c r="Q9">
-        <v>1388.6655483178949</v>
+        <v>1388.665548317895</v>
       </c>
       <c r="R9">
-        <v>1815.6633748481011</v>
+        <v>1815.663374848101</v>
       </c>
       <c r="S9">
-        <v>0.51476536531812866</v>
+        <v>0.5147653653181287</v>
       </c>
       <c r="U9">
-        <v>4.9402402723723933</v>
+        <v>4.940240272372393</v>
       </c>
       <c r="V9">
-        <v>0.51628619298192602</v>
+        <v>0.516286192981926</v>
       </c>
       <c r="W9">
-        <v>1.0295307306362571</v>
+        <v>1.029530730636257</v>
       </c>
       <c r="X9" t="s">
         <v>75</v>
@@ -1896,25 +1831,25 @@
         <v>60953</v>
       </c>
       <c r="AZ9">
-        <v>1325.0039999999999</v>
+        <v>1325.004</v>
       </c>
       <c r="BA9">
-        <v>0.99775583838271975</v>
+        <v>0.9977558383827198</v>
       </c>
       <c r="BB9" t="s">
         <v>83</v>
       </c>
       <c r="BC9">
-        <v>1150.5926086213169</v>
+        <v>1150.592608621317</v>
       </c>
       <c r="BD9">
-        <v>656.59159274116905</v>
+        <v>656.5915927411691</v>
       </c>
       <c r="BE9">
-        <v>404.73344537237477</v>
+        <v>404.7334453723748</v>
       </c>
     </row>
-    <row r="10" spans="1:60" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:60">
       <c r="A10" s="1">
         <v>8</v>
       </c>
@@ -1928,7 +1863,7 @@
         <v>67</v>
       </c>
       <c r="E10">
-        <v>103.28887227144401</v>
+        <v>103.288872271444</v>
       </c>
       <c r="F10">
         <v>1285.392850016151</v>
@@ -1940,10 +1875,10 @@
         <v>1285.392850016151</v>
       </c>
       <c r="I10">
-        <v>249.41132545137901</v>
+        <v>249.411325451379</v>
       </c>
       <c r="J10">
-        <v>0.61987033127605351</v>
+        <v>0.6198703312760535</v>
       </c>
       <c r="K10">
         <v>1.440147260087393</v>
@@ -1961,22 +1896,22 @@
         <v>1388.681722287595</v>
       </c>
       <c r="P10">
-        <v>296.13068511547363</v>
+        <v>296.1306851154736</v>
       </c>
       <c r="Q10">
         <v>1388.681722287595</v>
       </c>
       <c r="R10">
-        <v>390.84434904067098</v>
+        <v>390.844349040671</v>
       </c>
       <c r="S10">
-        <v>0.51447268935293522</v>
+        <v>0.5144726893529352</v>
       </c>
       <c r="U10">
-        <v>1.9340542741388911</v>
+        <v>1.934054274138891</v>
       </c>
       <c r="V10">
-        <v>0.53160816822661405</v>
+        <v>0.5316081682266141</v>
       </c>
       <c r="W10">
         <v>1.02894537870587</v>
@@ -2018,25 +1953,25 @@
         <v>61553</v>
       </c>
       <c r="AZ10">
-        <v>1325.0039999999999</v>
+        <v>1325.004</v>
       </c>
       <c r="BA10">
-        <v>0.99775763466419942</v>
+        <v>0.9977576346641994</v>
       </c>
       <c r="BB10" t="s">
         <v>84</v>
       </c>
       <c r="BC10">
-        <v>1150.5967463878069</v>
+        <v>1150.596746387807</v>
       </c>
       <c r="BD10">
         <v>119.2157097840018</v>
       </c>
       <c r="BE10">
-        <v>74.245003829273315</v>
+        <v>74.24500382927332</v>
       </c>
     </row>
-    <row r="11" spans="1:60" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:60">
       <c r="A11" s="1">
         <v>9</v>
       </c>
@@ -2056,7 +1991,7 @@
         <v>1285.470024130145</v>
       </c>
       <c r="G11">
-        <v>988.94480007205152</v>
+        <v>988.9448000720515</v>
       </c>
       <c r="H11">
         <v>1285.470074132646</v>
@@ -2065,16 +2000,16 @@
         <v>1433.106768375708</v>
       </c>
       <c r="J11">
-        <v>0.55266069975631194</v>
+        <v>0.5526606997563119</v>
       </c>
       <c r="K11">
-        <v>2.9183374160795079</v>
+        <v>2.918337416079508</v>
       </c>
       <c r="L11">
-        <v>0.58348740118428122</v>
+        <v>0.5834874011842812</v>
       </c>
       <c r="M11">
-        <v>1.1053213995126241</v>
+        <v>1.105321399512624</v>
       </c>
       <c r="N11" t="s">
         <v>75</v>
@@ -2089,55 +2024,55 @@
         <v>1388.769616085513</v>
       </c>
       <c r="R11">
-        <v>2265.3205312004611</v>
+        <v>2265.320531200461</v>
       </c>
       <c r="S11">
-        <v>0.48288952772712379</v>
+        <v>0.4828895277271238</v>
       </c>
       <c r="U11">
         <v>2.378189366748376</v>
       </c>
       <c r="V11">
-        <v>0.49346845382341792</v>
+        <v>0.4934684538234179</v>
       </c>
       <c r="W11">
-        <v>0.96577905545424758</v>
+        <v>0.9657790554542476</v>
       </c>
       <c r="X11" t="s">
         <v>75</v>
       </c>
       <c r="Y11">
-        <v>1265.2023824060441</v>
+        <v>1265.202382406044</v>
       </c>
       <c r="Z11">
         <v>102.332419393674</v>
       </c>
       <c r="AA11">
-        <v>0.80180413766771708</v>
+        <v>0.8018041376677171</v>
       </c>
       <c r="AB11">
-        <v>1410.1183612426289</v>
+        <v>1410.118361242629</v>
       </c>
       <c r="AC11">
-        <v>256.94610090791173</v>
+        <v>256.9461009079117</v>
       </c>
       <c r="AD11">
-        <v>0.61087061720005065</v>
+        <v>0.6108706172000506</v>
       </c>
       <c r="AE11">
-        <v>1370.6550569741819</v>
+        <v>1370.655056974182</v>
       </c>
       <c r="AF11">
-        <v>32.386778848817151</v>
+        <v>32.38677884881715</v>
       </c>
       <c r="AG11">
         <v>0.2393872087383124</v>
       </c>
       <c r="AH11">
-        <v>1381.5610010000059</v>
+        <v>1381.561001000006</v>
       </c>
       <c r="AI11">
-        <v>143.51899459075099</v>
+        <v>143.518994590751</v>
       </c>
       <c r="AJ11">
         <v>11.96955834124673</v>
@@ -2176,13 +2111,13 @@
         <v>47301</v>
       </c>
       <c r="AZ11">
-        <v>1325.0039999999999</v>
+        <v>1325.004</v>
       </c>
       <c r="BA11">
-        <v>0.99780473766019906</v>
+        <v>0.9978047376601991</v>
       </c>
     </row>
-    <row r="12" spans="1:60" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:60">
       <c r="A12" s="1">
         <v>10</v>
       </c>
@@ -2202,91 +2137,91 @@
         <v>1285.409241539194</v>
       </c>
       <c r="G12">
-        <v>815.58355708544991</v>
+        <v>815.5835570854499</v>
       </c>
       <c r="H12">
-        <v>1285.4092915416941</v>
+        <v>1285.409291541694</v>
       </c>
       <c r="I12">
         <v>1225.330054989565</v>
       </c>
       <c r="J12">
-        <v>0.55697069128529575</v>
+        <v>0.5569706912852957</v>
       </c>
       <c r="K12">
-        <v>2.3398825492268909</v>
+        <v>2.339882549226891</v>
       </c>
       <c r="L12">
         <v>0.6539941484020434</v>
       </c>
       <c r="M12">
-        <v>1.1139413825705911</v>
+        <v>1.113941382570591</v>
       </c>
       <c r="N12" t="s">
         <v>75</v>
       </c>
       <c r="O12">
-        <v>1388.7427245308261</v>
+        <v>1388.742724530826</v>
       </c>
       <c r="P12">
         <v>1533.610794844677</v>
       </c>
       <c r="Q12">
-        <v>1388.7427745333259</v>
+        <v>1388.742774533326</v>
       </c>
       <c r="R12">
         <v>1935.821413179566</v>
       </c>
       <c r="S12">
-        <v>0.49311025525220192</v>
+        <v>0.4931102552522019</v>
       </c>
       <c r="U12">
         <v>2.762318939681037</v>
       </c>
       <c r="V12">
-        <v>0.52752383266521607</v>
+        <v>0.5275238326652161</v>
       </c>
       <c r="W12">
-        <v>0.98622051050440374</v>
+        <v>0.9862205105044037</v>
       </c>
       <c r="X12" t="s">
         <v>75</v>
       </c>
       <c r="Y12">
-        <v>1265.2417638055399</v>
+        <v>1265.24176380554</v>
       </c>
       <c r="Z12">
         <v>101.2478021740942</v>
       </c>
       <c r="AA12">
-        <v>0.74630462001037912</v>
+        <v>0.7463046200103791</v>
       </c>
       <c r="AB12">
-        <v>1410.0777764046541</v>
+        <v>1410.077776404654</v>
       </c>
       <c r="AC12">
-        <v>231.29420724278299</v>
+        <v>231.294207242783</v>
       </c>
       <c r="AD12">
-        <v>0.71227034133365463</v>
+        <v>0.7122703413336546</v>
       </c>
       <c r="AE12">
         <v>1370.388723346935</v>
       </c>
       <c r="AF12">
-        <v>22.078433680098001</v>
+        <v>22.078433680098</v>
       </c>
       <c r="AG12">
-        <v>0.24517426831798031</v>
+        <v>0.2451742683179803</v>
       </c>
       <c r="AH12">
-        <v>1381.5610010000009</v>
+        <v>1381.561001000001</v>
       </c>
       <c r="AI12">
-        <v>111.41702371573039</v>
+        <v>111.4170237157304</v>
       </c>
       <c r="AJ12">
-        <v>12.259695127187101</v>
+        <v>12.2596951271871</v>
       </c>
       <c r="AN12" t="s">
         <v>69</v>
@@ -2322,13 +2257,13 @@
         <v>48438</v>
       </c>
       <c r="AZ12">
-        <v>1325.0039999999999</v>
+        <v>1325.004</v>
       </c>
       <c r="BA12">
-        <v>0.99779409982175749</v>
+        <v>0.9977940998217575</v>
       </c>
     </row>
-    <row r="13" spans="1:60" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:60">
       <c r="A13" s="1">
         <v>11</v>
       </c>
@@ -2348,52 +2283,52 @@
         <v>1285.401618508253</v>
       </c>
       <c r="G13">
-        <v>894.57727800272016</v>
+        <v>894.5772780027202</v>
       </c>
       <c r="H13">
         <v>1285.401668510754</v>
       </c>
       <c r="I13">
-        <v>1408.0364475926269</v>
+        <v>1408.036447592627</v>
       </c>
       <c r="J13">
-        <v>0.58730587841288207</v>
+        <v>0.5873058784128821</v>
       </c>
       <c r="K13">
         <v>2.730297314093431</v>
       </c>
       <c r="L13">
-        <v>0.63800162368659086</v>
+        <v>0.6380016236865909</v>
       </c>
       <c r="M13">
-        <v>1.1746117568257639</v>
+        <v>1.174611756825764</v>
       </c>
       <c r="N13" t="s">
         <v>75</v>
       </c>
       <c r="O13">
-        <v>1388.7082308787039</v>
+        <v>1388.708230878704</v>
       </c>
       <c r="P13">
-        <v>1645.3910751480921</v>
+        <v>1645.391075148092</v>
       </c>
       <c r="Q13">
         <v>1388.708280881204</v>
       </c>
       <c r="R13">
-        <v>2139.7445633437719</v>
+        <v>2139.744563343772</v>
       </c>
       <c r="S13">
-        <v>0.50495192392105093</v>
+        <v>0.5049519239210509</v>
       </c>
       <c r="U13">
-        <v>2.5012737967469971</v>
+        <v>2.501273796746997</v>
       </c>
       <c r="V13">
-        <v>0.54277120034537296</v>
+        <v>0.542771200345373</v>
       </c>
       <c r="W13">
-        <v>1.0099038478421021</v>
+        <v>1.009903847842102</v>
       </c>
       <c r="X13" t="s">
         <v>75</v>
@@ -2405,25 +2340,25 @@
         <v>118.4871160313557</v>
       </c>
       <c r="AA13">
-        <v>0.89509046278008486</v>
+        <v>0.8950904627800849</v>
       </c>
       <c r="AB13">
-        <v>1410.0302573003939</v>
+        <v>1410.030257300394</v>
       </c>
       <c r="AC13">
-        <v>247.60273827431459</v>
+        <v>247.6027382743146</v>
       </c>
       <c r="AD13">
-        <v>0.65079743686202141</v>
+        <v>0.6507974368620214</v>
       </c>
       <c r="AE13">
-        <v>1370.3261019051629</v>
+        <v>1370.326101905163</v>
       </c>
       <c r="AF13">
         <v>31.26164096369056</v>
       </c>
       <c r="AG13">
-        <v>0.25173599739308489</v>
+        <v>0.2517359973930849</v>
       </c>
       <c r="AH13">
         <v>1381.561001</v>
@@ -2468,10 +2403,10 @@
         <v>52620</v>
       </c>
       <c r="AZ13">
-        <v>1325.0039999999999</v>
+        <v>1325.004</v>
       </c>
       <c r="BA13">
-        <v>0.99776523583399068</v>
+        <v>0.9977652358339907</v>
       </c>
       <c r="BB13" t="s">
         <v>87</v>
@@ -2480,13 +2415,13 @@
         <v>1150.651543262938</v>
       </c>
       <c r="BD13">
-        <v>690.34754659504347</v>
+        <v>690.3475465950435</v>
       </c>
       <c r="BE13">
         <v>437.7999642504185</v>
       </c>
     </row>
-    <row r="14" spans="1:60" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:60">
       <c r="A14" s="1">
         <v>12</v>
       </c>
@@ -2503,34 +2438,34 @@
         <v>103.3006859854456</v>
       </c>
       <c r="F14">
-        <v>1285.3809567554431</v>
+        <v>1285.380956755443</v>
       </c>
       <c r="G14">
-        <v>1350.1033276976971</v>
+        <v>1350.103327697697</v>
       </c>
       <c r="H14">
-        <v>1285.3810067579429</v>
+        <v>1285.381006757943</v>
       </c>
       <c r="I14">
-        <v>2155.0657088306698</v>
+        <v>2155.06570883067</v>
       </c>
       <c r="J14">
-        <v>0.58619284871085675</v>
+        <v>0.5861928487108568</v>
       </c>
       <c r="K14">
         <v>2.606141576636285</v>
       </c>
       <c r="L14">
-        <v>0.67708738447575323</v>
+        <v>0.6770873844757532</v>
       </c>
       <c r="M14">
-        <v>1.1723856974217139</v>
+        <v>1.172385697421714</v>
       </c>
       <c r="N14" t="s">
         <v>75</v>
       </c>
       <c r="O14">
-        <v>1388.6816427408889</v>
+        <v>1388.681642740889</v>
       </c>
       <c r="P14">
         <v>2473.305295643419</v>
@@ -2542,13 +2477,13 @@
         <v>3252.660613804348</v>
       </c>
       <c r="S14">
-        <v>0.51367779261750823</v>
+        <v>0.5136777926175082</v>
       </c>
       <c r="U14">
-        <v>3.3754886565606639</v>
+        <v>3.375488656560664</v>
       </c>
       <c r="V14">
-        <v>0.52942229355326087</v>
+        <v>0.5294222935532609</v>
       </c>
       <c r="W14">
         <v>1.027355585235016</v>
@@ -2560,34 +2495,34 @@
         <v>1265.141748024909</v>
       </c>
       <c r="Z14">
-        <v>225.13291971659339</v>
+        <v>225.1329197165934</v>
       </c>
       <c r="AA14">
-        <v>0.75350462624827119</v>
+        <v>0.7535046262482712</v>
       </c>
       <c r="AB14">
-        <v>1410.0244989714511</v>
+        <v>1410.024498971451</v>
       </c>
       <c r="AC14">
-        <v>374.48810835902958</v>
+        <v>374.4881083590296</v>
       </c>
       <c r="AD14">
-        <v>0.65360496924864642</v>
+        <v>0.6536049692486464</v>
       </c>
       <c r="AE14">
         <v>1370.30903995832</v>
       </c>
       <c r="AF14">
-        <v>45.513263683679106</v>
+        <v>45.51326368367911</v>
       </c>
       <c r="AG14">
-        <v>0.25626631542494049</v>
+        <v>0.2562663154249405</v>
       </c>
       <c r="AH14">
         <v>1381.561001</v>
       </c>
       <c r="AI14">
-        <v>239.78993984137529</v>
+        <v>239.7899398413753</v>
       </c>
       <c r="AJ14">
         <v>12.8143446656447</v>
@@ -2626,25 +2561,25 @@
         <v>53534</v>
       </c>
       <c r="AZ14">
-        <v>1325.0039999999999</v>
+        <v>1325.004</v>
       </c>
       <c r="BA14">
-        <v>0.99776107645226009</v>
+        <v>0.9977610764522601</v>
       </c>
       <c r="BB14" t="s">
         <v>88</v>
       </c>
       <c r="BC14">
-        <v>1150.6140399995661</v>
+        <v>1150.614039999566</v>
       </c>
       <c r="BD14">
         <v>1181.442086529785</v>
       </c>
       <c r="BE14">
-        <v>738.91982644977668</v>
+        <v>738.9198264497767</v>
       </c>
     </row>
-    <row r="15" spans="1:60" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:60">
       <c r="A15" s="1">
         <v>13</v>
       </c>
@@ -2652,7 +2587,7 @@
         <v>0</v>
       </c>
       <c r="C15">
-        <v>103.02128647967059</v>
+        <v>103.0212864796706</v>
       </c>
       <c r="D15" t="s">
         <v>72</v>
@@ -2661,25 +2596,25 @@
         <v>103.2525911018095</v>
       </c>
       <c r="F15">
-        <v>1285.5869719932809</v>
+        <v>1285.586971993281</v>
       </c>
       <c r="G15">
-        <v>858.61965950073284</v>
+        <v>858.6196595007328</v>
       </c>
       <c r="H15">
         <v>1285.587021995781</v>
       </c>
       <c r="I15">
-        <v>1179.5101642360139</v>
+        <v>1179.510164236014</v>
       </c>
       <c r="J15">
         <v>0.5310479067236259</v>
       </c>
       <c r="K15">
-        <v>1.9972033414136521</v>
+        <v>1.997203341413652</v>
       </c>
       <c r="L15">
-        <v>0.54931728125298263</v>
+        <v>0.5493172812529826</v>
       </c>
       <c r="M15">
         <v>1.062095813447252</v>
@@ -2688,7 +2623,7 @@
         <v>75</v>
       </c>
       <c r="O15">
-        <v>1388.8395630950899</v>
+        <v>1388.83956309509</v>
       </c>
       <c r="P15">
         <v>1543.704491836095</v>
@@ -2700,55 +2635,55 @@
         <v>1808.138792200901</v>
       </c>
       <c r="S15">
-        <v>0.46264328604586302</v>
+        <v>0.462643286045863</v>
       </c>
       <c r="U15">
-        <v>2.2480755040772551</v>
+        <v>2.248075504077255</v>
       </c>
       <c r="V15">
-        <v>0.49757391779237209</v>
+        <v>0.4975739177923721</v>
       </c>
       <c r="W15">
-        <v>0.92528657209172605</v>
+        <v>0.925286572091726</v>
       </c>
       <c r="X15" t="s">
         <v>75</v>
       </c>
       <c r="Y15">
-        <v>1265.3366093029349</v>
+        <v>1265.336609302935</v>
       </c>
       <c r="Z15">
         <v>128.6822827375625</v>
       </c>
       <c r="AA15">
-        <v>0.71512951393903923</v>
+        <v>0.7151295139390392</v>
       </c>
       <c r="AB15">
-        <v>1410.1444181004199</v>
+        <v>1410.14441810042</v>
       </c>
       <c r="AC15">
-        <v>210.05021881922869</v>
+        <v>210.0502188192287</v>
       </c>
       <c r="AD15">
-        <v>0.60798832544962067</v>
+        <v>0.6079883254496207</v>
       </c>
       <c r="AE15">
-        <v>1371.9111376311009</v>
+        <v>1371.911137631101</v>
       </c>
       <c r="AF15">
-        <v>4.5590014834777222</v>
+        <v>4.559001483477722</v>
       </c>
       <c r="AG15">
-        <v>2.289472105412128E-2</v>
+        <v>0.02289472105412128</v>
       </c>
       <c r="AH15">
-        <v>1382.0917669999999</v>
+        <v>1382.091767</v>
       </c>
       <c r="AI15">
-        <v>77.871379952333427</v>
+        <v>77.87137995233343</v>
       </c>
       <c r="AJ15">
-        <v>11.442848066640259</v>
+        <v>11.44284806664026</v>
       </c>
       <c r="AN15" t="s">
         <v>72</v>
@@ -2784,13 +2719,13 @@
         <v>53850</v>
       </c>
       <c r="AZ15">
-        <v>1325.0039999999999</v>
+        <v>1325.004</v>
       </c>
       <c r="BA15">
-        <v>0.99775981774722933</v>
+        <v>0.9977598177472293</v>
       </c>
     </row>
-    <row r="16" spans="1:60" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:60">
       <c r="A16" s="1">
         <v>14</v>
       </c>
@@ -2798,7 +2733,7 @@
         <v>0</v>
       </c>
       <c r="C16">
-        <v>103.07371948291529</v>
+        <v>103.0737194829153</v>
       </c>
       <c r="D16" t="s">
         <v>73</v>
@@ -2807,52 +2742,52 @@
         <v>103.305631911044</v>
       </c>
       <c r="F16">
-        <v>1285.3737791614551</v>
+        <v>1285.373779161455</v>
       </c>
       <c r="G16">
-        <v>997.88350354002603</v>
+        <v>997.883503540026</v>
       </c>
       <c r="H16">
         <v>1285.373829163955</v>
       </c>
       <c r="I16">
-        <v>1565.9064619498799</v>
+        <v>1565.90646194988</v>
       </c>
       <c r="J16">
-        <v>0.59087129629348845</v>
+        <v>0.5908712962934884</v>
       </c>
       <c r="K16">
-        <v>3.1781651815198999</v>
+        <v>3.1781651815199</v>
       </c>
       <c r="L16">
-        <v>0.61556371486072037</v>
+        <v>0.6155637148607204</v>
       </c>
       <c r="M16">
-        <v>1.1817425925869769</v>
+        <v>1.181742592586977</v>
       </c>
       <c r="N16" t="s">
         <v>75</v>
       </c>
       <c r="O16">
-        <v>1388.6794110724991</v>
+        <v>1388.679411072499</v>
       </c>
       <c r="P16">
         <v>1878.232856316419</v>
       </c>
       <c r="Q16">
-        <v>1388.6794610749989</v>
+        <v>1388.679461074999</v>
       </c>
       <c r="R16">
-        <v>2457.1983839794002</v>
+        <v>2457.1983839794</v>
       </c>
       <c r="S16">
-        <v>0.51330857828160126</v>
+        <v>0.5133085782816013</v>
       </c>
       <c r="U16">
-        <v>2.8086744290190842</v>
+        <v>2.808674429019084</v>
       </c>
       <c r="V16">
-        <v>0.51956484380938261</v>
+        <v>0.5195648438093826</v>
       </c>
       <c r="W16">
         <v>1.026617156563203</v>
@@ -2861,22 +2796,22 @@
         <v>75</v>
       </c>
       <c r="Y16">
-        <v>1265.1097526908729</v>
+        <v>1265.109752690873</v>
       </c>
       <c r="Z16">
-        <v>140.10172117792879</v>
+        <v>140.1017211779288</v>
       </c>
       <c r="AA16">
-        <v>0.85031433475853579</v>
+        <v>0.8503143347585358</v>
       </c>
       <c r="AB16">
         <v>1410.011320886817</v>
       </c>
       <c r="AC16">
-        <v>292.22927895439949</v>
+        <v>292.2292789543995</v>
       </c>
       <c r="AD16">
-        <v>0.67181571272173957</v>
+        <v>0.6718157127217396</v>
       </c>
       <c r="AE16">
         <v>1370.324388795583</v>
@@ -2885,13 +2820,13 @@
         <v>31.63658531573078</v>
       </c>
       <c r="AG16">
-        <v>0.25597200337442622</v>
+        <v>0.2559720033744262</v>
       </c>
       <c r="AH16">
         <v>1382.309524834963</v>
       </c>
       <c r="AI16">
-        <v>222.76623494209679</v>
+        <v>222.7662349420968</v>
       </c>
       <c r="AJ16">
         <v>12.80167952399977</v>
@@ -2930,7 +2865,7 @@
         <v>60661</v>
       </c>
       <c r="AZ16">
-        <v>1325.0039999999999</v>
+        <v>1325.004</v>
       </c>
       <c r="BA16">
         <v>0.9977550843662768</v>
@@ -2939,16 +2874,16 @@
         <v>90</v>
       </c>
       <c r="BC16">
-        <v>1150.6097053009571</v>
+        <v>1150.609705300957</v>
       </c>
       <c r="BD16">
-        <v>840.54119080356531</v>
+        <v>840.5411908035653</v>
       </c>
       <c r="BE16">
-        <v>506.83940566423303</v>
+        <v>506.839405664233</v>
       </c>
     </row>
-    <row r="17" spans="1:57" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:57">
       <c r="A17" s="1">
         <v>15</v>
       </c>
@@ -2965,16 +2900,16 @@
         <v>103.307474445164</v>
       </c>
       <c r="F17">
-        <v>1285.3416492006399</v>
+        <v>1285.34164920064</v>
       </c>
       <c r="G17">
-        <v>1184.5676023766421</v>
+        <v>1184.567602376642</v>
       </c>
       <c r="H17">
         <v>1285.34169920314</v>
       </c>
       <c r="I17">
-        <v>1945.2584406522119</v>
+        <v>1945.258440652212</v>
       </c>
       <c r="J17">
         <v>0.6049970384885992</v>
@@ -2983,7 +2918,7 @@
         <v>2.982766416196478</v>
       </c>
       <c r="L17">
-        <v>0.66938351186394673</v>
+        <v>0.6693835118639467</v>
       </c>
       <c r="M17">
         <v>1.209994076977198</v>
@@ -2992,7 +2927,7 @@
         <v>75</v>
       </c>
       <c r="O17">
-        <v>1388.6491236458039</v>
+        <v>1388.649123645804</v>
       </c>
       <c r="P17">
         <v>2189.315646431859</v>
@@ -3001,58 +2936,58 @@
         <v>1388.649173648304</v>
       </c>
       <c r="R17">
-        <v>2893.3801296106199</v>
+        <v>2893.38012961062</v>
       </c>
       <c r="S17">
-        <v>0.51158149445316825</v>
+        <v>0.5115814944531683</v>
       </c>
       <c r="U17">
-        <v>3.1593286107656362</v>
+        <v>3.159328610765636</v>
       </c>
       <c r="V17">
-        <v>0.55165341779863086</v>
+        <v>0.5516534177986309</v>
       </c>
       <c r="W17">
-        <v>1.0231629889063369</v>
+        <v>1.023162988906337</v>
       </c>
       <c r="X17" t="s">
         <v>75</v>
       </c>
       <c r="Y17">
-        <v>1265.1010747032431</v>
+        <v>1265.101074703243</v>
       </c>
       <c r="Z17">
-        <v>219.47365245010761</v>
+        <v>219.4736524501076</v>
       </c>
       <c r="AA17">
-        <v>0.86140580115292342</v>
+        <v>0.8614058011529234</v>
       </c>
       <c r="AB17">
-        <v>1410.0100341853561</v>
+        <v>1410.010034185356</v>
       </c>
       <c r="AC17">
-        <v>346.21650636803821</v>
+        <v>346.2165063680382</v>
       </c>
       <c r="AD17">
-        <v>0.67129692149409448</v>
+        <v>0.6712969214940945</v>
       </c>
       <c r="AE17">
         <v>1370.283040968576</v>
       </c>
       <c r="AF17">
-        <v>40.974215945510778</v>
+        <v>40.97421594551078</v>
       </c>
       <c r="AG17">
-        <v>0.25553900624688008</v>
+        <v>0.2555390062468801</v>
       </c>
       <c r="AH17">
         <v>1381.561001000003</v>
       </c>
       <c r="AI17">
-        <v>184.11111197891651</v>
+        <v>184.1111119789165</v>
       </c>
       <c r="AJ17">
-        <v>12.777628919374891</v>
+        <v>12.77762891937489</v>
       </c>
       <c r="AN17" t="s">
         <v>74</v>
@@ -3088,7 +3023,7 @@
         <v>61234</v>
       </c>
       <c r="AZ17">
-        <v>1325.0039999999999</v>
+        <v>1325.004</v>
       </c>
       <c r="BA17">
         <v>0.9977566382832278</v>
@@ -3100,10 +3035,10 @@
         <v>1150.57139130514</v>
       </c>
       <c r="BD17">
-        <v>1175.3689870695041</v>
+        <v>1175.368987069504</v>
       </c>
       <c r="BE17">
-        <v>735.48093744728124</v>
+        <v>735.4809374472812</v>
       </c>
     </row>
   </sheetData>

</xml_diff>